<commit_message>
Added Summer 2025 folder: User_interface_v2 is the developing function for the user framework. Currently, it is able to allow user to load the user-defined functions, specify the part of the test that requires assumptions of normality, assesses for normality based on the user's answer, and then performed the appropriate downstream procedure based on the results of the normality test.
</commit_message>
<xml_diff>
--- a/Simulation/TYPE I ERROR/OneSampleTypeI.errorRate_2step.xlsx
+++ b/Simulation/TYPE I ERROR/OneSampleTypeI.errorRate_2step.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -426,34 +426,34 @@
         </is>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.241</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.19</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.278</v>
       </c>
       <c r="E2">
-        <v>0.2</v>
+        <v>0.267</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.121</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.145</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.146</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.157</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>0.172</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>0.334</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -468,34 +468,34 @@
         </is>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.292</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.265</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.347</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.314</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.132</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>0.222</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>0.227</v>
       </c>
       <c r="I3">
-        <v>0.2</v>
+        <v>0.216</v>
       </c>
       <c r="J3">
-        <v>0.4</v>
+        <v>0.233</v>
       </c>
       <c r="K3">
-        <v>0.2</v>
+        <v>0.531</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -510,34 +510,34 @@
         </is>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.438</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.413</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.474</v>
       </c>
       <c r="E4">
-        <v>0.2</v>
+        <v>0.442</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.167</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>0.365</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>0.376</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>0.412</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>0.404</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>0.729</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
@@ -552,34 +552,34 @@
         </is>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.574</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.54</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.606</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.608</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.233</v>
       </c>
       <c r="G5">
-        <v>0.2</v>
+        <v>0.464</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>0.469</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>0.546</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>0.859</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -594,34 +594,34 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.2</v>
+        <v>0.67</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.641</v>
       </c>
       <c r="D6">
-        <v>0.4</v>
+        <v>0.704</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.657</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.281</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>0.542</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="I6">
-        <v>0.2</v>
+        <v>0.623</v>
       </c>
       <c r="J6">
-        <v>0.2</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>0.929</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -636,80 +636,38 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.2</v>
+        <v>0.739</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.722</v>
       </c>
       <c r="D7">
-        <v>0.2</v>
+        <v>0.794</v>
       </c>
       <c r="E7">
-        <v>0.2</v>
+        <v>0.769</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.324</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>0.638</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>0.636</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>0.708</v>
       </c>
       <c r="J7">
-        <v>0.2</v>
+        <v>0.666</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>0.971</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>30</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0.2</v>
-      </c>
-      <c r="E8">
-        <v>0.2</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0.4</v>
-      </c>
-      <c r="H8">
-        <v>0.2</v>
-      </c>
-      <c r="I8">
-        <v>0.2</v>
-      </c>
-      <c r="J8">
-        <v>0.6</v>
-      </c>
-      <c r="K8">
-        <v>0.4</v>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>50</t>
         </is>
       </c>
     </row>

</xml_diff>